<commit_message>
made revisions specific to lab 7
</commit_message>
<xml_diff>
--- a/Labs/Lab07/CS133JS_Lab07_Rubric.xlsx
+++ b/Labs/Lab07/CS133JS_Lab07_Rubric.xlsx
@@ -1,41 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CS133JS-CourseMaterials\Labs\Lab06\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS133JS-CourseMaterials/Labs/Lab07/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3665FB-5270-4C48-A440-820086BEA250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1219F571-B3C9-FF4E-87E2-607B6C9B124D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33660" yWindow="4260" windowWidth="17628" windowHeight="12024" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
+    <workbookView xWindow="12520" yWindow="500" windowWidth="13080" windowHeight="14560" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Criteria</t>
   </si>
@@ -67,28 +57,34 @@
     <t>Style and best practices</t>
   </si>
   <si>
-    <t>Grading Rubric for Lab 6: Objects</t>
-  </si>
-  <si>
     <t>Object exercises</t>
   </si>
   <si>
-    <t>Web app functionality</t>
-  </si>
-  <si>
-    <t>Array declaration</t>
-  </si>
-  <si>
-    <t>Function parameters, return value</t>
-  </si>
-  <si>
-    <t>Object constructor</t>
-  </si>
-  <si>
-    <t>Check for valid index range</t>
-  </si>
-  <si>
-    <t>Functions required to return success status (true/false)</t>
+    <t>Grading Rubric for Lab 7: Events</t>
+  </si>
+  <si>
+    <t>Web app I functionality</t>
+  </si>
+  <si>
+    <t>Web App I: Average Calculator, Cost Per Mile Calc, Temperature conversion</t>
+  </si>
+  <si>
+    <t>Web App II: : Multiple-choice quiz, true-false quiz, fill-in-the-blank quiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">document.querySelector used </t>
+  </si>
+  <si>
+    <t>Web app II functionality</t>
+  </si>
+  <si>
+    <t>Click-event calls a function</t>
+  </si>
+  <si>
+    <t>Input elements and button for input</t>
+  </si>
+  <si>
+    <t>Event handler function</t>
   </si>
 </sst>
 </file>
@@ -465,20 +461,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3216228F-B421-8943-9C69-C9FAC1E7C520}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="3" max="3" width="22.796875" customWidth="1"/>
+    <col min="1" max="1" width="3" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -509,7 +506,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="4">
         <v>10</v>
@@ -541,43 +538,43 @@
         <v>12</v>
       </c>
       <c r="D9" s="4">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E9" s="4">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>13</v>
+      <c r="B10" t="s">
+        <v>18</v>
       </c>
       <c r="D10" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E10" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>14</v>
+      <c r="B11" t="s">
+        <v>17</v>
       </c>
       <c r="D11" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E11" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>15</v>
+      <c r="B12" t="s">
+        <v>19</v>
       </c>
       <c r="D12" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E12" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -585,56 +582,99 @@
         <v>16</v>
       </c>
       <c r="D13" s="4">
+        <v>6</v>
+      </c>
+      <c r="E13" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="4">
+        <v>4</v>
+      </c>
+      <c r="E14" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="4">
+        <v>4</v>
+      </c>
+      <c r="E16" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="4">
         <v>2</v>
       </c>
-      <c r="E13" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="4">
-        <v>2</v>
-      </c>
-      <c r="E14" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="4">
-        <v>5</v>
-      </c>
-      <c r="E15" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="4">
-        <v>2</v>
-      </c>
-      <c r="E16" s="4">
+      <c r="E17" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="4">
+        <v>5</v>
+      </c>
+      <c r="E18" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="4">
+        <v>2</v>
+      </c>
+      <c r="E19" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
         <v>3</v>
       </c>
-      <c r="D18">
-        <f>SUM(D6:D16)</f>
+      <c r="D21">
+        <f>SUM(D6:D19)</f>
         <v>50</v>
       </c>
-      <c r="E18">
-        <f>SUM(E6:E16)</f>
+      <c r="E21">
+        <f>SUM(E6:E19)</f>
         <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the lab 7 rubric
</commit_message>
<xml_diff>
--- a/Labs/Lab07/CS133JS_Lab07_Rubric.xlsx
+++ b/Labs/Lab07/CS133JS_Lab07_Rubric.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CS133JS-CourseMaterials\Labs\Lab07\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brian/Repos/CS133JS-CourseMaterials/Labs/Lab07/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F16049-8C3E-4DE7-88A9-CDD0F202053E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCA4164-1707-5346-B0AE-160614DB5065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19212" yWindow="4308" windowWidth="17556" windowHeight="11592" activeTab="1" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="26240" windowHeight="15420" activeTab="1" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
   <si>
     <t>Criteria</t>
   </si>
@@ -115,12 +115,24 @@
   </si>
   <si>
     <t>(MPG)</t>
+  </si>
+  <si>
+    <t>Price per gallon</t>
+  </si>
+  <si>
+    <t>Excellent work!</t>
+  </si>
+  <si>
+    <t>Here's the grade breakdown:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="5">
     <font>
       <sz val="12"/>
@@ -177,12 +189,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -201,9 +220,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -241,7 +260,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -347,7 +366,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -489,7 +508,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -503,11 +522,11 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="3" max="3" width="22.796875" customWidth="1"/>
-    <col min="6" max="6" width="16.796875" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -675,18 +694,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14151F0F-FB94-6846-92DC-36F755BDEC5D}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="41.09765625" customWidth="1"/>
-    <col min="3" max="3" width="8.19921875" customWidth="1"/>
-    <col min="4" max="4" width="5.69921875" customWidth="1"/>
+    <col min="2" max="2" width="41.1640625" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" customWidth="1"/>
     <col min="5" max="5" width="2.5" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
   </cols>
@@ -702,234 +721,280 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="1"/>
+      <c r="A3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="A4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="3" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>8</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="2" t="s">
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
+      <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>4</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10">
-        <v>3</v>
-      </c>
-      <c r="D10">
-        <v>3</v>
-      </c>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6">
       <c r="B11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D11">
-        <v>1</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:6">
       <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-      <c r="D12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>5</v>
       </c>
-      <c r="D13">
+      <c r="D14">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="B14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14">
-        <v>3</v>
-      </c>
-      <c r="D14">
-        <v>3</v>
-      </c>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:6">
       <c r="B15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D15">
-        <v>1</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:6">
       <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="B17" t="s">
         <v>19</v>
       </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-      <c r="D16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="B17" t="s">
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="B18" t="s">
         <v>15</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>2</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" t="s">
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
         <v>9</v>
       </c>
-      <c r="C18">
-        <v>3</v>
-      </c>
-      <c r="D18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" t="s">
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
         <v>7</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>2</v>
       </c>
-      <c r="D19">
+      <c r="D20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21">
-        <f>SUM(C6:C19)</f>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <f>SUM(C7:C20)</f>
         <v>40</v>
       </c>
-      <c r="D21">
-        <f>SUM(D6:D19)</f>
+      <c r="D22">
+        <f>SUM(D7:D20)</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" t="s">
+      <c r="F22" s="6"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
-      <c r="B24" t="s">
+    <row r="25" spans="1:8">
+      <c r="B25" t="s">
         <v>24</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>22</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>23</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F25" t="s">
+        <v>26</v>
+      </c>
+      <c r="G25" t="s">
         <v>21</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H25" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
-      <c r="C25">
+    <row r="26" spans="1:8">
+      <c r="C26">
         <v>300</v>
       </c>
-      <c r="D25">
+      <c r="D26">
         <v>10</v>
       </c>
-      <c r="F25" t="e">
-        <f>#REF! * D25 / C25</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G25">
-        <f>C25/D25</f>
+      <c r="F26">
+        <v>4</v>
+      </c>
+      <c r="G26" s="5">
+        <f>F26 * D26 / C26</f>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="H26">
+        <f>C26/D26</f>
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
-      <c r="A26" t="s">
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added best practice separation of i/o from processing
</commit_message>
<xml_diff>
--- a/Labs/Lab07/CS133JS_Lab07_Rubric.xlsx
+++ b/Labs/Lab07/CS133JS_Lab07_Rubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brian/Repos/CS133JS-CourseMaterials/Labs/Lab07/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCA4164-1707-5346-B0AE-160614DB5065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BB3B3C-7995-2C43-9E39-4F4A7EF3BEDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="26240" windowHeight="15420" activeTab="1" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
   <si>
     <t>Criteria</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>Here's the grade breakdown:</t>
+  </si>
+  <si>
+    <t>Style and best practices (separation of i/o)</t>
   </si>
 </sst>
 </file>
@@ -199,7 +202,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -696,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14151F0F-FB94-6846-92DC-36F755BDEC5D}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
@@ -902,7 +905,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C19">
         <v>3</v>

</xml_diff>